<commit_message>
Update Project Report and Add LR Study
</commit_message>
<xml_diff>
--- a/Literature Review/Similar Systems.xlsx
+++ b/Literature Review/Similar Systems.xlsx
@@ -19,12 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="77">
   <si>
     <t>#</t>
-  </si>
-  <si>
-    <t>Feasibility Study</t>
   </si>
   <si>
     <t>Yes</t>
@@ -107,18 +104,9 @@
     <t>Disaster monitoring</t>
   </si>
   <si>
-    <t>Conflict tracking</t>
-  </si>
-  <si>
-    <t>Crime tracking</t>
-  </si>
-  <si>
     <t xml:space="preserve"> News tracking</t>
   </si>
   <si>
-    <t>AI-powered insights</t>
-  </si>
-  <si>
     <t>User-reported data</t>
   </si>
   <si>
@@ -146,12 +134,6 @@
     <t>c16</t>
   </si>
   <si>
-    <t>Custom filters</t>
-  </si>
-  <si>
-    <t>Sources</t>
-  </si>
-  <si>
     <t>Liveuamap.com</t>
   </si>
   <si>
@@ -210,13 +192,91 @@
   </si>
   <si>
     <t>crimemapping.com</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes By Againcies</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>Yes | Ukrain</t>
+  </si>
+  <si>
+    <t>Yes |USA</t>
+  </si>
+  <si>
+    <t>Syria, Iraq</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9 out of 16</t>
+  </si>
+  <si>
+    <t>Yes | USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10 out of 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6 out of 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12 out of 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5 out of 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7 out of 16</t>
+  </si>
+  <si>
+    <t>Ukrain</t>
+  </si>
+  <si>
+    <t>Yes |Ukrain</t>
+  </si>
+  <si>
+    <t>Conflict monitoring</t>
+  </si>
+  <si>
+    <t>Yes |UN</t>
+  </si>
+  <si>
+    <t>Yes |Hungarin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 13 out of 16</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>Crime monitoring</t>
+  </si>
+  <si>
+    <t>Using Web Crawlers</t>
+  </si>
+  <si>
+    <t>Custom filters on Data</t>
+  </si>
+  <si>
+    <t>Similar System Review Study</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,8 +319,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -297,8 +371,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6E0B4"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBDD7EE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -330,6 +434,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -351,9 +468,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -363,13 +477,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -386,9 +496,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -401,40 +508,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -445,20 +520,76 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -740,31 +871,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:CA128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="S24" sqref="D2:T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="6.1796875" customWidth="1"/>
     <col min="3" max="3" width="9.1796875" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" customWidth="1"/>
-    <col min="5" max="5" width="23.7265625" customWidth="1"/>
+    <col min="4" max="4" width="5.54296875" customWidth="1"/>
+    <col min="5" max="5" width="23.26953125" customWidth="1"/>
     <col min="6" max="6" width="16.81640625" customWidth="1"/>
-    <col min="7" max="7" width="13.7265625" customWidth="1"/>
-    <col min="8" max="8" width="23.6328125" customWidth="1"/>
-    <col min="9" max="9" width="8.7265625" customWidth="1"/>
-    <col min="10" max="10" width="21.1796875" customWidth="1"/>
-    <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="20.453125" customWidth="1"/>
-    <col min="13" max="13" width="11.26953125" customWidth="1"/>
-    <col min="14" max="14" width="18.08984375" customWidth="1"/>
+    <col min="7" max="7" width="15.36328125" customWidth="1"/>
+    <col min="8" max="8" width="22.54296875" customWidth="1"/>
+    <col min="9" max="9" width="17.7265625" customWidth="1"/>
+    <col min="10" max="10" width="22" customWidth="1"/>
+    <col min="11" max="11" width="17.7265625" customWidth="1"/>
+    <col min="12" max="12" width="15.453125" customWidth="1"/>
+    <col min="13" max="13" width="21.81640625" customWidth="1"/>
+    <col min="14" max="14" width="15" customWidth="1"/>
     <col min="15" max="15" width="14.7265625" customWidth="1"/>
-    <col min="16" max="16" width="11.7265625" customWidth="1"/>
+    <col min="16" max="16" width="14.1796875" customWidth="1"/>
     <col min="17" max="17" width="16.90625" customWidth="1"/>
-    <col min="18" max="18" width="15.08984375" customWidth="1"/>
+    <col min="18" max="18" width="14.26953125" customWidth="1"/>
     <col min="19" max="19" width="20.81640625" customWidth="1"/>
     <col min="20" max="20" width="17.6328125" customWidth="1"/>
     <col min="21" max="21" width="13.453125" customWidth="1"/>
@@ -822,38 +956,38 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
+      <c r="D2" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
       <c r="U2" s="38"/>
       <c r="V2" s="38"/>
       <c r="W2" s="38"/>
       <c r="X2" s="38"/>
       <c r="Y2" s="38"/>
       <c r="Z2" s="38"/>
-      <c r="AA2" s="42"/>
-      <c r="AB2" s="42"/>
-      <c r="AC2" s="42"/>
-      <c r="AD2" s="42"/>
-      <c r="AE2" s="42"/>
-      <c r="AF2" s="42"/>
-      <c r="AG2" s="42"/>
+      <c r="AA2" s="24"/>
+      <c r="AB2" s="24"/>
+      <c r="AC2" s="24"/>
+      <c r="AD2" s="24"/>
+      <c r="AE2" s="24"/>
+      <c r="AF2" s="24"/>
+      <c r="AG2" s="24"/>
       <c r="AH2" s="2"/>
       <c r="AI2" s="2"/>
       <c r="AJ2" s="2"/>
@@ -864,38 +998,38 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="36"/>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="36"/>
-      <c r="R3" s="36"/>
-      <c r="S3" s="36"/>
-      <c r="T3" s="36"/>
-      <c r="U3" s="36"/>
-      <c r="V3" s="36"/>
-      <c r="W3" s="36"/>
-      <c r="X3" s="36"/>
-      <c r="Y3" s="36"/>
-      <c r="Z3" s="36"/>
-      <c r="AA3" s="43"/>
-      <c r="AB3" s="43"/>
-      <c r="AC3" s="43"/>
-      <c r="AD3" s="43"/>
-      <c r="AE3" s="43"/>
-      <c r="AF3" s="43"/>
-      <c r="AG3" s="43"/>
+      <c r="D3" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="33"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="33"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="39"/>
+      <c r="Z3" s="39"/>
+      <c r="AA3" s="25"/>
+      <c r="AB3" s="25"/>
+      <c r="AC3" s="25"/>
+      <c r="AD3" s="25"/>
+      <c r="AE3" s="25"/>
+      <c r="AF3" s="25"/>
+      <c r="AG3" s="25"/>
       <c r="AH3" s="2"/>
       <c r="AI3" s="2"/>
       <c r="AJ3" s="2"/>
@@ -906,36 +1040,36 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="37"/>
-      <c r="S4" s="37"/>
-      <c r="T4" s="37"/>
-      <c r="U4" s="37"/>
-      <c r="V4" s="37"/>
-      <c r="W4" s="37"/>
-      <c r="X4" s="37"/>
-      <c r="Y4" s="37"/>
-      <c r="Z4" s="37"/>
-      <c r="AA4" s="43"/>
-      <c r="AB4" s="43"/>
-      <c r="AC4" s="43"/>
-      <c r="AD4" s="43"/>
-      <c r="AE4" s="43"/>
-      <c r="AF4" s="43"/>
-      <c r="AG4" s="43"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="34"/>
+      <c r="S4" s="34"/>
+      <c r="T4" s="34"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="25"/>
+      <c r="X4" s="25"/>
+      <c r="Y4" s="25"/>
+      <c r="Z4" s="25"/>
+      <c r="AA4" s="25"/>
+      <c r="AB4" s="25"/>
+      <c r="AC4" s="25"/>
+      <c r="AD4" s="25"/>
+      <c r="AE4" s="25"/>
+      <c r="AF4" s="25"/>
+      <c r="AG4" s="25"/>
       <c r="AH4" s="2"/>
       <c r="AI4" s="2"/>
       <c r="AJ4" s="2"/>
@@ -946,68 +1080,68 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="31" t="s">
+      <c r="N5" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="O5" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="P5" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="K5" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="L5" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="M5" s="31" t="s">
+      <c r="Q5" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="R5" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="N5" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="O5" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="P5" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q5" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="R5" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="S5" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="T5" s="31"/>
-      <c r="U5" s="31"/>
-      <c r="V5" s="31"/>
-      <c r="W5" s="31"/>
-      <c r="X5" s="31"/>
-      <c r="Y5" s="31"/>
-      <c r="Z5" s="31"/>
-      <c r="AA5" s="32"/>
-      <c r="AB5" s="32"/>
-      <c r="AC5" s="32"/>
-      <c r="AD5" s="32"/>
-      <c r="AE5" s="32"/>
-      <c r="AF5" s="32"/>
-      <c r="AG5" s="32"/>
+      <c r="S5" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="T5" s="43"/>
+      <c r="U5" s="35"/>
+      <c r="V5" s="35"/>
+      <c r="W5" s="13"/>
+      <c r="X5" s="13"/>
+      <c r="Y5" s="13"/>
+      <c r="Z5" s="13"/>
+      <c r="AA5" s="13"/>
+      <c r="AB5" s="13"/>
+      <c r="AC5" s="13"/>
+      <c r="AD5" s="13"/>
+      <c r="AE5" s="13"/>
+      <c r="AF5" s="23"/>
+      <c r="AG5" s="23"/>
       <c r="AH5" s="2"/>
       <c r="AI5" s="2"/>
       <c r="AJ5" s="2"/>
@@ -1018,42 +1152,68 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
-      <c r="W6" s="10"/>
-      <c r="X6" s="10"/>
-      <c r="Y6" s="10"/>
-      <c r="Z6" s="10"/>
-      <c r="AA6" s="18"/>
-      <c r="AB6" s="18"/>
-      <c r="AC6" s="18"/>
-      <c r="AD6" s="18"/>
-      <c r="AE6" s="23"/>
-      <c r="AF6" s="23"/>
-      <c r="AG6" s="18"/>
+      <c r="D6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="O6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q6" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="R6" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="S6" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="T6" s="9"/>
+      <c r="U6" s="36"/>
+      <c r="V6" s="36"/>
+      <c r="W6" s="13"/>
+      <c r="X6" s="13"/>
+      <c r="Y6" s="13"/>
+      <c r="Z6" s="13"/>
+      <c r="AA6" s="50"/>
+      <c r="AB6" s="13"/>
+      <c r="AC6" s="13"/>
+      <c r="AD6" s="13"/>
+      <c r="AE6" s="13"/>
+      <c r="AF6" s="18"/>
+      <c r="AG6" s="13"/>
       <c r="AH6" s="2"/>
       <c r="AI6" s="2"/>
       <c r="AJ6" s="2"/>
@@ -1064,42 +1224,68 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="F7" s="34"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="41"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11"/>
-      <c r="W7" s="11"/>
-      <c r="X7" s="11"/>
-      <c r="Y7" s="11"/>
-      <c r="Z7" s="11"/>
-      <c r="AA7" s="18"/>
-      <c r="AB7" s="18"/>
-      <c r="AC7" s="18"/>
-      <c r="AD7" s="18"/>
-      <c r="AE7" s="23"/>
-      <c r="AF7" s="44"/>
-      <c r="AG7" s="18"/>
+      <c r="D7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L7" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q7" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="R7" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="T7" s="42"/>
+      <c r="U7" s="36"/>
+      <c r="V7" s="36"/>
+      <c r="W7" s="13"/>
+      <c r="X7" s="13"/>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="13"/>
+      <c r="AA7" s="13"/>
+      <c r="AB7" s="13"/>
+      <c r="AC7" s="13"/>
+      <c r="AD7" s="13"/>
+      <c r="AE7" s="13"/>
+      <c r="AF7" s="26"/>
+      <c r="AG7" s="13"/>
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
       <c r="AJ7" s="2"/>
@@ -1110,40 +1296,68 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
-      <c r="W8" s="10"/>
-      <c r="X8" s="10"/>
-      <c r="Y8" s="10"/>
-      <c r="Z8" s="10"/>
-      <c r="AA8" s="18"/>
-      <c r="AB8" s="18"/>
-      <c r="AC8" s="18"/>
-      <c r="AD8" s="18"/>
-      <c r="AE8" s="18"/>
-      <c r="AF8" s="44"/>
-      <c r="AG8" s="18"/>
+      <c r="D8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="L8" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="N8" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="O8" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="P8" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q8" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="R8" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="S8" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="T8" s="9"/>
+      <c r="U8" s="36"/>
+      <c r="V8" s="36"/>
+      <c r="W8" s="13"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="13"/>
+      <c r="Z8" s="13"/>
+      <c r="AA8" s="13"/>
+      <c r="AB8" s="13"/>
+      <c r="AC8" s="13"/>
+      <c r="AD8" s="13"/>
+      <c r="AE8" s="13"/>
+      <c r="AF8" s="26"/>
+      <c r="AG8" s="13"/>
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
       <c r="AJ8" s="2"/>
@@ -1154,40 +1368,68 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="34"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
-      <c r="W9" s="11"/>
-      <c r="X9" s="11"/>
-      <c r="Y9" s="11"/>
-      <c r="Z9" s="11"/>
-      <c r="AA9" s="18"/>
-      <c r="AB9" s="18"/>
-      <c r="AC9" s="18"/>
-      <c r="AD9" s="18"/>
-      <c r="AE9" s="44"/>
-      <c r="AF9" s="44"/>
-      <c r="AG9" s="18"/>
+      <c r="D9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="L9" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="O9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="P9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q9" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="R9" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="S9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="T9" s="10"/>
+      <c r="U9" s="36"/>
+      <c r="V9" s="36"/>
+      <c r="W9" s="13"/>
+      <c r="X9" s="13"/>
+      <c r="Y9" s="13"/>
+      <c r="Z9" s="13"/>
+      <c r="AA9" s="13"/>
+      <c r="AB9" s="13"/>
+      <c r="AC9" s="13"/>
+      <c r="AD9" s="13"/>
+      <c r="AE9" s="13"/>
+      <c r="AF9" s="26"/>
+      <c r="AG9" s="13"/>
       <c r="AH9" s="2"/>
       <c r="AI9" s="2"/>
       <c r="AJ9" s="2"/>
@@ -1198,40 +1440,68 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="33"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
-      <c r="V10" s="10"/>
-      <c r="W10" s="10"/>
-      <c r="X10" s="10"/>
-      <c r="Y10" s="10"/>
-      <c r="Z10" s="10"/>
-      <c r="AA10" s="18"/>
-      <c r="AB10" s="18"/>
-      <c r="AC10" s="18"/>
-      <c r="AD10" s="18"/>
-      <c r="AE10" s="44"/>
-      <c r="AF10" s="44"/>
-      <c r="AG10" s="18"/>
+      <c r="D10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="L10" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="O10" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="P10" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="R10" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="S10" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="T10" s="9"/>
+      <c r="U10" s="36"/>
+      <c r="V10" s="36"/>
+      <c r="W10" s="13"/>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="13"/>
+      <c r="AA10" s="13"/>
+      <c r="AB10" s="13"/>
+      <c r="AC10" s="13"/>
+      <c r="AD10" s="13"/>
+      <c r="AE10" s="13"/>
+      <c r="AF10" s="26"/>
+      <c r="AG10" s="13"/>
       <c r="AH10" s="2"/>
       <c r="AI10" s="2"/>
       <c r="AJ10" s="2"/>
@@ -1242,40 +1512,68 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="34"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
-      <c r="U11" s="11"/>
-      <c r="V11" s="11"/>
-      <c r="W11" s="11"/>
-      <c r="X11" s="11"/>
-      <c r="Y11" s="11"/>
-      <c r="Z11" s="11"/>
-      <c r="AA11" s="18"/>
-      <c r="AB11" s="18"/>
-      <c r="AC11" s="18"/>
-      <c r="AD11" s="18"/>
-      <c r="AE11" s="45"/>
-      <c r="AF11" s="23"/>
-      <c r="AG11" s="18"/>
+      <c r="D11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="N11" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="O11" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="P11" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q11" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="R11" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="S11" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="T11" s="10"/>
+      <c r="U11" s="36"/>
+      <c r="V11" s="36"/>
+      <c r="W11" s="13"/>
+      <c r="X11" s="13"/>
+      <c r="Y11" s="13"/>
+      <c r="Z11" s="13"/>
+      <c r="AA11" s="13"/>
+      <c r="AB11" s="13"/>
+      <c r="AC11" s="13"/>
+      <c r="AD11" s="13"/>
+      <c r="AE11" s="13"/>
+      <c r="AF11" s="18"/>
+      <c r="AG11" s="13"/>
       <c r="AH11" s="2"/>
       <c r="AI11" s="2"/>
       <c r="AJ11" s="2"/>
@@ -1286,40 +1584,68 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="33"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
-      <c r="S12" s="10"/>
-      <c r="T12" s="10"/>
-      <c r="U12" s="10"/>
-      <c r="V12" s="10"/>
-      <c r="W12" s="10"/>
-      <c r="X12" s="10"/>
-      <c r="Y12" s="10"/>
-      <c r="Z12" s="10"/>
-      <c r="AA12" s="18"/>
-      <c r="AB12" s="18"/>
-      <c r="AC12" s="18"/>
-      <c r="AD12" s="18"/>
-      <c r="AE12" s="44"/>
-      <c r="AF12" s="44"/>
-      <c r="AG12" s="18"/>
+      <c r="D12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="L12" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="N12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="R12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="S12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="T12" s="9"/>
+      <c r="U12" s="36"/>
+      <c r="V12" s="36"/>
+      <c r="W12" s="13"/>
+      <c r="X12" s="13"/>
+      <c r="Y12" s="13"/>
+      <c r="Z12" s="13"/>
+      <c r="AA12" s="13"/>
+      <c r="AB12" s="13"/>
+      <c r="AC12" s="13"/>
+      <c r="AD12" s="13"/>
+      <c r="AE12" s="13"/>
+      <c r="AF12" s="26"/>
+      <c r="AG12" s="13"/>
       <c r="AH12" s="2"/>
       <c r="AI12" s="2"/>
       <c r="AJ12" s="2"/>
@@ -1330,40 +1656,68 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="34"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="11"/>
-      <c r="U13" s="11"/>
-      <c r="V13" s="11"/>
-      <c r="W13" s="11"/>
-      <c r="X13" s="11"/>
-      <c r="Y13" s="11"/>
-      <c r="Z13" s="11"/>
-      <c r="AA13" s="18"/>
-      <c r="AB13" s="18"/>
-      <c r="AC13" s="18"/>
-      <c r="AD13" s="18"/>
-      <c r="AE13" s="45"/>
-      <c r="AF13" s="23"/>
-      <c r="AG13" s="18"/>
+      <c r="D13" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="L13" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="N13" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="O13" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="P13" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="R13" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="S13" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="T13" s="10"/>
+      <c r="U13" s="36"/>
+      <c r="V13" s="36"/>
+      <c r="W13" s="13"/>
+      <c r="X13" s="13"/>
+      <c r="Y13" s="13"/>
+      <c r="Z13" s="13"/>
+      <c r="AA13" s="13"/>
+      <c r="AB13" s="13"/>
+      <c r="AC13" s="13"/>
+      <c r="AD13" s="13"/>
+      <c r="AE13" s="13"/>
+      <c r="AF13" s="18"/>
+      <c r="AG13" s="13"/>
       <c r="AH13" s="2"/>
       <c r="AI13" s="2"/>
       <c r="AJ13" s="2"/>
@@ -1374,40 +1728,68 @@
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="35"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="27"/>
-      <c r="N14" s="27"/>
-      <c r="O14" s="27"/>
-      <c r="P14" s="27"/>
-      <c r="Q14" s="27"/>
-      <c r="R14" s="27"/>
-      <c r="S14" s="27"/>
-      <c r="T14" s="27"/>
-      <c r="U14" s="27"/>
-      <c r="V14" s="27"/>
+      <c r="D14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="J14" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="K14" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="L14" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="M14" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="N14" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="O14" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="P14" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q14" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="R14" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="S14" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="T14" s="21"/>
+      <c r="U14" s="36"/>
+      <c r="V14" s="36"/>
       <c r="W14" s="27"/>
       <c r="X14" s="27"/>
-      <c r="Y14" s="27"/>
+      <c r="Y14" s="13"/>
       <c r="Z14" s="27"/>
-      <c r="AA14" s="46"/>
-      <c r="AB14" s="46"/>
-      <c r="AC14" s="46"/>
-      <c r="AD14" s="46"/>
-      <c r="AE14" s="47"/>
-      <c r="AF14" s="47"/>
-      <c r="AG14" s="46"/>
+      <c r="AA14" s="27"/>
+      <c r="AB14" s="27"/>
+      <c r="AC14" s="27"/>
+      <c r="AD14" s="27"/>
+      <c r="AE14" s="27"/>
+      <c r="AF14" s="28"/>
+      <c r="AG14" s="27"/>
       <c r="AH14" s="2"/>
       <c r="AI14" s="2"/>
       <c r="AJ14" s="2"/>
@@ -1418,40 +1800,68 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="29"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="28"/>
-      <c r="Q15" s="29"/>
-      <c r="R15" s="29"/>
-      <c r="S15" s="29"/>
-      <c r="T15" s="29"/>
-      <c r="U15" s="29"/>
-      <c r="V15" s="29"/>
-      <c r="W15" s="29"/>
-      <c r="X15" s="29"/>
-      <c r="Y15" s="17"/>
-      <c r="Z15" s="17"/>
-      <c r="AA15" s="2"/>
-      <c r="AB15" s="2"/>
-      <c r="AC15" s="2"/>
-      <c r="AD15" s="2"/>
-      <c r="AE15" s="44"/>
-      <c r="AF15" s="44"/>
-      <c r="AG15" s="18"/>
+      <c r="D15" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="L15" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="N15" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="O15" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="P15" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q15" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="R15" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="S15" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="T15" s="10"/>
+      <c r="U15" s="37"/>
+      <c r="V15" s="37"/>
+      <c r="W15" s="13"/>
+      <c r="X15" s="13"/>
+      <c r="Y15" s="13"/>
+      <c r="Z15" s="13"/>
+      <c r="AA15" s="13"/>
+      <c r="AB15" s="13"/>
+      <c r="AC15" s="13"/>
+      <c r="AD15" s="13"/>
+      <c r="AE15" s="13"/>
+      <c r="AF15" s="26"/>
+      <c r="AG15" s="13"/>
       <c r="AH15" s="2"/>
       <c r="AI15" s="2"/>
       <c r="AJ15" s="2"/>
@@ -1462,40 +1872,68 @@
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="35"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="49"/>
-      <c r="N16" s="50"/>
-      <c r="O16" s="27"/>
-      <c r="P16" s="27"/>
-      <c r="Q16" s="50"/>
-      <c r="R16" s="50"/>
-      <c r="S16" s="50"/>
-      <c r="T16" s="50"/>
-      <c r="U16" s="50"/>
-      <c r="V16" s="50"/>
-      <c r="W16" s="50"/>
-      <c r="X16" s="50"/>
-      <c r="Y16" s="30"/>
-      <c r="Z16" s="30"/>
-      <c r="AA16" s="48"/>
-      <c r="AB16" s="48"/>
-      <c r="AC16" s="48"/>
-      <c r="AD16" s="48"/>
-      <c r="AE16" s="47"/>
-      <c r="AF16" s="47"/>
-      <c r="AG16" s="46"/>
+      <c r="D16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="L16" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="M16" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="N16" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="O16" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="P16" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q16" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="R16" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="S16" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="T16" s="21"/>
+      <c r="U16" s="37"/>
+      <c r="V16" s="37"/>
+      <c r="W16" s="27"/>
+      <c r="X16" s="27"/>
+      <c r="Y16" s="13"/>
+      <c r="Z16" s="27"/>
+      <c r="AA16" s="27"/>
+      <c r="AB16" s="27"/>
+      <c r="AC16" s="27"/>
+      <c r="AD16" s="27"/>
+      <c r="AE16" s="27"/>
+      <c r="AF16" s="28"/>
+      <c r="AG16" s="27"/>
       <c r="AH16" s="2"/>
       <c r="AI16" s="2"/>
       <c r="AJ16" s="2"/>
@@ -1506,38 +1944,68 @@
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
-      <c r="S17" s="11"/>
-      <c r="T17" s="11"/>
-      <c r="U17" s="29"/>
-      <c r="V17" s="29"/>
-      <c r="W17" s="29"/>
-      <c r="X17" s="29"/>
-      <c r="Y17" s="17"/>
-      <c r="Z17" s="17"/>
-      <c r="AA17" s="2"/>
-      <c r="AB17" s="2"/>
-      <c r="AC17" s="2"/>
-      <c r="AD17" s="2"/>
-      <c r="AE17" s="44"/>
-      <c r="AF17" s="44"/>
-      <c r="AG17" s="18"/>
+      <c r="D17" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="L17" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="M17" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="N17" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="O17" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="P17" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q17" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="R17" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="S17" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="T17" s="10"/>
+      <c r="U17" s="37"/>
+      <c r="V17" s="37"/>
+      <c r="W17" s="13"/>
+      <c r="X17" s="13"/>
+      <c r="Y17" s="13"/>
+      <c r="Z17" s="13"/>
+      <c r="AA17" s="13"/>
+      <c r="AB17" s="13"/>
+      <c r="AC17" s="13"/>
+      <c r="AD17" s="13"/>
+      <c r="AE17" s="13"/>
+      <c r="AF17" s="26"/>
+      <c r="AG17" s="13"/>
       <c r="AH17" s="2"/>
       <c r="AI17" s="2"/>
       <c r="AJ17" s="2"/>
@@ -1548,40 +2016,68 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="35"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="49"/>
-      <c r="N18" s="50"/>
-      <c r="O18" s="27"/>
-      <c r="P18" s="27"/>
-      <c r="Q18" s="50"/>
-      <c r="R18" s="50"/>
-      <c r="S18" s="50"/>
-      <c r="T18" s="50"/>
-      <c r="U18" s="50"/>
-      <c r="V18" s="50"/>
-      <c r="W18" s="50"/>
-      <c r="X18" s="50"/>
-      <c r="Y18" s="30"/>
-      <c r="Z18" s="30"/>
-      <c r="AA18" s="2"/>
-      <c r="AB18" s="2"/>
-      <c r="AC18" s="2"/>
-      <c r="AD18" s="2"/>
-      <c r="AE18" s="44"/>
-      <c r="AF18" s="44"/>
-      <c r="AG18" s="18"/>
+      <c r="D18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="I18" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="L18" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="M18" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="N18" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="O18" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="P18" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q18" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="R18" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="S18" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="T18" s="21"/>
+      <c r="U18" s="37"/>
+      <c r="V18" s="37"/>
+      <c r="W18" s="27"/>
+      <c r="X18" s="27"/>
+      <c r="Y18" s="13"/>
+      <c r="Z18" s="27"/>
+      <c r="AA18" s="27"/>
+      <c r="AB18" s="27"/>
+      <c r="AC18" s="27"/>
+      <c r="AD18" s="27"/>
+      <c r="AE18" s="27"/>
+      <c r="AF18" s="26"/>
+      <c r="AG18" s="13"/>
       <c r="AH18" s="2"/>
       <c r="AI18" s="2"/>
       <c r="AJ18" s="2"/>
@@ -1592,40 +2088,68 @@
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" s="34"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="11"/>
-      <c r="S19" s="11"/>
-      <c r="T19" s="11"/>
-      <c r="U19" s="29"/>
-      <c r="V19" s="29"/>
-      <c r="W19" s="29"/>
-      <c r="X19" s="29"/>
-      <c r="Y19" s="17"/>
-      <c r="Z19" s="17"/>
-      <c r="AA19" s="2"/>
-      <c r="AB19" s="2"/>
-      <c r="AC19" s="2"/>
-      <c r="AD19" s="2"/>
-      <c r="AE19" s="44"/>
-      <c r="AF19" s="44"/>
-      <c r="AG19" s="18"/>
+      <c r="D19" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="L19" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="M19" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="N19" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="O19" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="P19" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q19" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="R19" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="S19" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="T19" s="10"/>
+      <c r="U19" s="37"/>
+      <c r="V19" s="37"/>
+      <c r="W19" s="13"/>
+      <c r="X19" s="13"/>
+      <c r="Y19" s="13"/>
+      <c r="Z19" s="13"/>
+      <c r="AA19" s="13"/>
+      <c r="AB19" s="13"/>
+      <c r="AC19" s="13"/>
+      <c r="AD19" s="13"/>
+      <c r="AE19" s="13"/>
+      <c r="AF19" s="26"/>
+      <c r="AG19" s="13"/>
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
       <c r="AJ19" s="2"/>
@@ -1636,40 +2160,68 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" s="33"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
-      <c r="S20" s="15"/>
-      <c r="T20" s="15"/>
-      <c r="U20" s="15"/>
-      <c r="V20" s="15"/>
-      <c r="W20" s="15"/>
-      <c r="X20" s="15"/>
-      <c r="Y20" s="16"/>
-      <c r="Z20" s="16"/>
-      <c r="AA20" s="2"/>
-      <c r="AB20" s="2"/>
-      <c r="AC20" s="2"/>
-      <c r="AD20" s="2"/>
-      <c r="AE20" s="44"/>
-      <c r="AF20" s="44"/>
-      <c r="AG20" s="18"/>
+      <c r="D20" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L20" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="M20" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="N20" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="O20" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="P20" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="R20" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="S20" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="T20" s="9"/>
+      <c r="U20" s="37"/>
+      <c r="V20" s="37"/>
+      <c r="W20" s="13"/>
+      <c r="X20" s="13"/>
+      <c r="Y20" s="13"/>
+      <c r="Z20" s="13"/>
+      <c r="AA20" s="13"/>
+      <c r="AB20" s="13"/>
+      <c r="AC20" s="13"/>
+      <c r="AD20" s="23"/>
+      <c r="AE20" s="13"/>
+      <c r="AF20" s="26"/>
+      <c r="AG20" s="13"/>
       <c r="AH20" s="2"/>
       <c r="AI20" s="2"/>
       <c r="AJ20" s="2"/>
@@ -1680,40 +2232,68 @@
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="F21" s="34"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="29"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="29"/>
-      <c r="R21" s="29"/>
-      <c r="S21" s="29"/>
-      <c r="T21" s="29"/>
-      <c r="U21" s="29"/>
-      <c r="V21" s="29"/>
-      <c r="W21" s="29"/>
-      <c r="X21" s="29"/>
-      <c r="Y21" s="17"/>
-      <c r="Z21" s="17"/>
-      <c r="AA21" s="2"/>
-      <c r="AB21" s="2"/>
-      <c r="AC21" s="2"/>
-      <c r="AD21" s="2"/>
-      <c r="AE21" s="44"/>
-      <c r="AF21" s="44"/>
-      <c r="AG21" s="18"/>
+      <c r="D21" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H21" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="L21" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="M21" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="N21" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="O21" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="P21" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="R21" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="S21" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="T21" s="10"/>
+      <c r="U21" s="37"/>
+      <c r="V21" s="37"/>
+      <c r="W21" s="13"/>
+      <c r="X21" s="13"/>
+      <c r="Y21" s="13"/>
+      <c r="Z21" s="13"/>
+      <c r="AA21" s="13"/>
+      <c r="AB21" s="13"/>
+      <c r="AC21" s="13"/>
+      <c r="AD21" s="23"/>
+      <c r="AE21" s="13"/>
+      <c r="AF21" s="26"/>
+      <c r="AG21" s="13"/>
       <c r="AH21" s="2"/>
       <c r="AI21" s="2"/>
       <c r="AJ21" s="2"/>
@@ -1724,38 +2304,36 @@
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="F22" s="34"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="29"/>
-      <c r="O22" s="11"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="29"/>
-      <c r="R22" s="29"/>
-      <c r="S22" s="29"/>
-      <c r="T22" s="29"/>
-      <c r="U22" s="29"/>
-      <c r="V22" s="29"/>
-      <c r="W22" s="29"/>
-      <c r="X22" s="29"/>
-      <c r="Y22" s="17"/>
-      <c r="Z22" s="17"/>
-      <c r="AA22" s="2"/>
-      <c r="AB22" s="2"/>
-      <c r="AC22" s="2"/>
-      <c r="AD22" s="2"/>
-      <c r="AE22" s="2"/>
+      <c r="D22" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="16"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="37"/>
+      <c r="V22" s="37"/>
+      <c r="W22" s="13"/>
+      <c r="X22" s="13"/>
+      <c r="Y22" s="13"/>
+      <c r="Z22" s="13"/>
+      <c r="AA22" s="13"/>
+      <c r="AB22" s="13"/>
+      <c r="AC22" s="13"/>
+      <c r="AD22" s="13"/>
+      <c r="AE22" s="13"/>
       <c r="AF22" s="2"/>
       <c r="AG22" s="2"/>
       <c r="AH22" s="2"/>
@@ -1768,38 +2346,36 @@
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="F23" s="34"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="28"/>
-      <c r="N23" s="29"/>
-      <c r="O23" s="11"/>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="29"/>
-      <c r="R23" s="29"/>
-      <c r="S23" s="29"/>
-      <c r="T23" s="29"/>
-      <c r="U23" s="29"/>
-      <c r="V23" s="29"/>
-      <c r="W23" s="29"/>
-      <c r="X23" s="29"/>
-      <c r="Y23" s="17"/>
-      <c r="Z23" s="17"/>
-      <c r="AA23" s="2"/>
-      <c r="AB23" s="2"/>
-      <c r="AC23" s="2"/>
-      <c r="AD23" s="2"/>
-      <c r="AE23" s="2"/>
+      <c r="D23" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="15"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="47"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="22"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="22"/>
+      <c r="U23" s="37"/>
+      <c r="V23" s="37"/>
+      <c r="W23" s="13"/>
+      <c r="X23" s="13"/>
+      <c r="Y23" s="23"/>
+      <c r="Z23" s="13"/>
+      <c r="AA23" s="13"/>
+      <c r="AB23" s="13"/>
+      <c r="AC23" s="23"/>
+      <c r="AD23" s="23"/>
+      <c r="AE23" s="13"/>
       <c r="AF23" s="2"/>
       <c r="AG23" s="2"/>
       <c r="AH23" s="2"/>
@@ -1808,38 +2384,70 @@
       <c r="AK23" s="2"/>
       <c r="AL23" s="2"/>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:38" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="14"/>
-      <c r="T24" s="14"/>
+      <c r="D24" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="H24" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="I24" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="J24" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="K24" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="L24" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="M24" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="N24" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="O24" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="P24" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q24" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="R24" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="S24" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="T24" s="41"/>
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
-      <c r="W24" s="2"/>
-      <c r="X24" s="2"/>
-      <c r="Y24" s="2"/>
-      <c r="Z24" s="2"/>
-      <c r="AA24" s="2"/>
-      <c r="AB24" s="2"/>
-      <c r="AC24" s="2"/>
-      <c r="AD24" s="2"/>
-      <c r="AE24" s="2"/>
+      <c r="W24" s="13"/>
+      <c r="X24" s="13"/>
+      <c r="Y24" s="13"/>
+      <c r="Z24" s="13"/>
+      <c r="AA24" s="13"/>
+      <c r="AB24" s="13"/>
+      <c r="AC24" s="13"/>
+      <c r="AD24" s="13"/>
+      <c r="AE24" s="13"/>
       <c r="AF24" s="2"/>
       <c r="AG24" s="2"/>
       <c r="AH24" s="2"/>
@@ -1853,22 +2461,22 @@
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="6"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
       <c r="K25" s="8"/>
       <c r="L25" s="7"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="14"/>
-      <c r="Q25" s="14"/>
-      <c r="R25" s="14"/>
-      <c r="S25" s="14"/>
-      <c r="T25" s="14"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="12"/>
+      <c r="T25" s="12"/>
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
       <c r="W25" s="2"/>
@@ -1893,22 +2501,22 @@
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="6"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
       <c r="K26" s="8"/>
       <c r="L26" s="7"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
-      <c r="T26" s="14"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
+      <c r="T26" s="12"/>
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
       <c r="W26" s="2"/>
@@ -1933,22 +2541,22 @@
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="6"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
       <c r="K27" s="8"/>
       <c r="L27" s="7"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
-      <c r="T27" s="14"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="12"/>
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
       <c r="W27" s="2"/>
@@ -1973,12 +2581,12 @@
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="6"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
       <c r="K28" s="8"/>
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
@@ -2013,22 +2621,22 @@
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="6"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
       <c r="K29" s="8"/>
       <c r="L29" s="7"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="14"/>
-      <c r="Q29" s="14"/>
-      <c r="R29" s="14"/>
-      <c r="S29" s="14"/>
-      <c r="T29" s="14"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="12"/>
+      <c r="S29" s="12"/>
+      <c r="T29" s="12"/>
       <c r="U29" s="2"/>
       <c r="V29" s="2"/>
       <c r="W29" s="2"/>
@@ -2055,20 +2663,20 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
       <c r="K30" s="7"/>
       <c r="L30" s="7"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="14"/>
-      <c r="Q30" s="14"/>
-      <c r="R30" s="14"/>
-      <c r="S30" s="14"/>
-      <c r="T30" s="14"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
+      <c r="R30" s="12"/>
+      <c r="S30" s="12"/>
+      <c r="T30" s="12"/>
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
       <c r="W30" s="2"/>
@@ -2101,14 +2709,14 @@
       <c r="J31" s="6"/>
       <c r="K31" s="7"/>
       <c r="L31" s="7"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="14"/>
-      <c r="P31" s="14"/>
-      <c r="Q31" s="14"/>
-      <c r="R31" s="14"/>
-      <c r="S31" s="14"/>
-      <c r="T31" s="14"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="12"/>
+      <c r="R31" s="12"/>
+      <c r="S31" s="12"/>
+      <c r="T31" s="12"/>
       <c r="U31" s="2"/>
       <c r="V31" s="2"/>
       <c r="W31" s="2"/>
@@ -2141,14 +2749,14 @@
       <c r="J32" s="6"/>
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
-      <c r="P32" s="14"/>
-      <c r="Q32" s="14"/>
-      <c r="R32" s="14"/>
-      <c r="S32" s="14"/>
-      <c r="T32" s="14"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="12"/>
+      <c r="O32" s="12"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="12"/>
+      <c r="R32" s="12"/>
+      <c r="S32" s="12"/>
+      <c r="T32" s="12"/>
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
       <c r="W32" s="2"/>
@@ -2181,14 +2789,14 @@
       <c r="J33" s="6"/>
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14"/>
-      <c r="P33" s="14"/>
-      <c r="Q33" s="14"/>
-      <c r="R33" s="14"/>
-      <c r="S33" s="14"/>
-      <c r="T33" s="14"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="12"/>
+      <c r="Q33" s="12"/>
+      <c r="R33" s="12"/>
+      <c r="S33" s="12"/>
+      <c r="T33" s="12"/>
       <c r="U33" s="2"/>
       <c r="V33" s="2"/>
       <c r="W33" s="2"/>
@@ -2248,28 +2856,28 @@
       <c r="AK34" s="2"/>
       <c r="AL34" s="2"/>
       <c r="BI34" t="s">
+        <v>2</v>
+      </c>
+      <c r="BJ34" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="BJ34" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="BK34" s="40"/>
-      <c r="BL34" s="40"/>
-      <c r="BM34" s="40"/>
-      <c r="BN34" s="40"/>
-      <c r="BO34" s="40"/>
-      <c r="BP34" s="19"/>
-      <c r="BQ34" s="19"/>
-      <c r="BR34" s="19"/>
-      <c r="BS34" s="19"/>
-      <c r="BT34" s="19"/>
-      <c r="BU34" s="19"/>
-      <c r="BV34" s="19"/>
-      <c r="BW34" s="19"/>
-      <c r="BX34" s="19"/>
-      <c r="BY34" s="19"/>
-      <c r="BZ34" s="19"/>
-      <c r="CA34" s="19"/>
+      <c r="BK34" s="31"/>
+      <c r="BL34" s="31"/>
+      <c r="BM34" s="31"/>
+      <c r="BN34" s="31"/>
+      <c r="BO34" s="31"/>
+      <c r="BP34" s="14"/>
+      <c r="BQ34" s="14"/>
+      <c r="BR34" s="14"/>
+      <c r="BS34" s="14"/>
+      <c r="BT34" s="14"/>
+      <c r="BU34" s="14"/>
+      <c r="BV34" s="14"/>
+      <c r="BW34" s="14"/>
+      <c r="BX34" s="14"/>
+      <c r="BY34" s="14"/>
+      <c r="BZ34" s="14"/>
+      <c r="CA34" s="14"/>
     </row>
     <row r="35" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
@@ -2284,14 +2892,14 @@
       <c r="J35" s="6"/>
       <c r="K35" s="7"/>
       <c r="L35" s="7"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14"/>
-      <c r="P35" s="14"/>
-      <c r="Q35" s="14"/>
-      <c r="R35" s="14"/>
-      <c r="S35" s="14"/>
-      <c r="T35" s="14"/>
+      <c r="M35" s="12"/>
+      <c r="N35" s="12"/>
+      <c r="O35" s="12"/>
+      <c r="P35" s="12"/>
+      <c r="Q35" s="12"/>
+      <c r="R35" s="12"/>
+      <c r="S35" s="12"/>
+      <c r="T35" s="12"/>
       <c r="U35" s="2"/>
       <c r="V35" s="2"/>
       <c r="W35" s="2"/>
@@ -2305,24 +2913,24 @@
       <c r="AE35" s="2"/>
       <c r="AF35" s="2"/>
       <c r="AG35" s="2"/>
-      <c r="BJ35" s="40"/>
-      <c r="BK35" s="40"/>
-      <c r="BL35" s="40"/>
-      <c r="BM35" s="40"/>
-      <c r="BN35" s="40"/>
-      <c r="BO35" s="40"/>
-      <c r="BP35" s="19"/>
-      <c r="BQ35" s="19"/>
-      <c r="BR35" s="19"/>
-      <c r="BS35" s="19"/>
-      <c r="BT35" s="19"/>
-      <c r="BU35" s="19"/>
-      <c r="BV35" s="19"/>
-      <c r="BW35" s="19"/>
-      <c r="BX35" s="19"/>
-      <c r="BY35" s="19"/>
-      <c r="BZ35" s="19"/>
-      <c r="CA35" s="19"/>
+      <c r="BJ35" s="31"/>
+      <c r="BK35" s="31"/>
+      <c r="BL35" s="31"/>
+      <c r="BM35" s="31"/>
+      <c r="BN35" s="31"/>
+      <c r="BO35" s="31"/>
+      <c r="BP35" s="14"/>
+      <c r="BQ35" s="14"/>
+      <c r="BR35" s="14"/>
+      <c r="BS35" s="14"/>
+      <c r="BT35" s="14"/>
+      <c r="BU35" s="14"/>
+      <c r="BV35" s="14"/>
+      <c r="BW35" s="14"/>
+      <c r="BX35" s="14"/>
+      <c r="BY35" s="14"/>
+      <c r="BZ35" s="14"/>
+      <c r="CA35" s="14"/>
     </row>
     <row r="36" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
@@ -2358,24 +2966,24 @@
       <c r="AE36" s="2"/>
       <c r="AF36" s="2"/>
       <c r="AG36" s="2"/>
-      <c r="BJ36" s="40"/>
-      <c r="BK36" s="40"/>
-      <c r="BL36" s="40"/>
-      <c r="BM36" s="40"/>
-      <c r="BN36" s="40"/>
-      <c r="BO36" s="40"/>
-      <c r="BP36" s="19"/>
-      <c r="BQ36" s="19"/>
-      <c r="BR36" s="19"/>
-      <c r="BS36" s="19"/>
-      <c r="BT36" s="19"/>
-      <c r="BU36" s="19"/>
-      <c r="BV36" s="19"/>
-      <c r="BW36" s="19"/>
-      <c r="BX36" s="19"/>
-      <c r="BY36" s="19"/>
-      <c r="BZ36" s="19"/>
-      <c r="CA36" s="19"/>
+      <c r="BJ36" s="31"/>
+      <c r="BK36" s="31"/>
+      <c r="BL36" s="31"/>
+      <c r="BM36" s="31"/>
+      <c r="BN36" s="31"/>
+      <c r="BO36" s="31"/>
+      <c r="BP36" s="14"/>
+      <c r="BQ36" s="14"/>
+      <c r="BR36" s="14"/>
+      <c r="BS36" s="14"/>
+      <c r="BT36" s="14"/>
+      <c r="BU36" s="14"/>
+      <c r="BV36" s="14"/>
+      <c r="BW36" s="14"/>
+      <c r="BX36" s="14"/>
+      <c r="BY36" s="14"/>
+      <c r="BZ36" s="14"/>
+      <c r="CA36" s="14"/>
     </row>
     <row r="37" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
@@ -2411,24 +3019,24 @@
       <c r="AE37" s="2"/>
       <c r="AF37" s="2"/>
       <c r="AG37" s="2"/>
-      <c r="BJ37" s="40"/>
-      <c r="BK37" s="40"/>
-      <c r="BL37" s="40"/>
-      <c r="BM37" s="40"/>
-      <c r="BN37" s="40"/>
-      <c r="BO37" s="40"/>
-      <c r="BP37" s="19"/>
-      <c r="BQ37" s="19"/>
-      <c r="BR37" s="19"/>
-      <c r="BS37" s="19"/>
-      <c r="BT37" s="19"/>
-      <c r="BU37" s="19"/>
-      <c r="BV37" s="19"/>
-      <c r="BW37" s="19"/>
-      <c r="BX37" s="19"/>
-      <c r="BY37" s="19"/>
-      <c r="BZ37" s="19"/>
-      <c r="CA37" s="19"/>
+      <c r="BJ37" s="31"/>
+      <c r="BK37" s="31"/>
+      <c r="BL37" s="31"/>
+      <c r="BM37" s="31"/>
+      <c r="BN37" s="31"/>
+      <c r="BO37" s="31"/>
+      <c r="BP37" s="14"/>
+      <c r="BQ37" s="14"/>
+      <c r="BR37" s="14"/>
+      <c r="BS37" s="14"/>
+      <c r="BT37" s="14"/>
+      <c r="BU37" s="14"/>
+      <c r="BV37" s="14"/>
+      <c r="BW37" s="14"/>
+      <c r="BX37" s="14"/>
+      <c r="BY37" s="14"/>
+      <c r="BZ37" s="14"/>
+      <c r="CA37" s="14"/>
     </row>
     <row r="38" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
@@ -2464,24 +3072,24 @@
       <c r="AE38" s="2"/>
       <c r="AF38" s="2"/>
       <c r="AG38" s="2"/>
-      <c r="BJ38" s="40"/>
-      <c r="BK38" s="40"/>
-      <c r="BL38" s="40"/>
-      <c r="BM38" s="40"/>
-      <c r="BN38" s="40"/>
-      <c r="BO38" s="40"/>
-      <c r="BP38" s="19"/>
-      <c r="BQ38" s="19"/>
-      <c r="BR38" s="19"/>
-      <c r="BS38" s="19"/>
-      <c r="BT38" s="19"/>
-      <c r="BU38" s="19"/>
-      <c r="BV38" s="19"/>
-      <c r="BW38" s="19"/>
-      <c r="BX38" s="19"/>
-      <c r="BY38" s="19"/>
-      <c r="BZ38" s="19"/>
-      <c r="CA38" s="19"/>
+      <c r="BJ38" s="31"/>
+      <c r="BK38" s="31"/>
+      <c r="BL38" s="31"/>
+      <c r="BM38" s="31"/>
+      <c r="BN38" s="31"/>
+      <c r="BO38" s="31"/>
+      <c r="BP38" s="14"/>
+      <c r="BQ38" s="14"/>
+      <c r="BR38" s="14"/>
+      <c r="BS38" s="14"/>
+      <c r="BT38" s="14"/>
+      <c r="BU38" s="14"/>
+      <c r="BV38" s="14"/>
+      <c r="BW38" s="14"/>
+      <c r="BX38" s="14"/>
+      <c r="BY38" s="14"/>
+      <c r="BZ38" s="14"/>
+      <c r="CA38" s="14"/>
     </row>
     <row r="39" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
@@ -2517,24 +3125,24 @@
       <c r="AE39" s="2"/>
       <c r="AF39" s="2"/>
       <c r="AG39" s="2"/>
-      <c r="BJ39" s="40"/>
-      <c r="BK39" s="40"/>
-      <c r="BL39" s="40"/>
-      <c r="BM39" s="40"/>
-      <c r="BN39" s="40"/>
-      <c r="BO39" s="40"/>
-      <c r="BP39" s="19"/>
-      <c r="BQ39" s="19"/>
-      <c r="BR39" s="19"/>
-      <c r="BS39" s="19"/>
-      <c r="BT39" s="19"/>
-      <c r="BU39" s="19"/>
-      <c r="BV39" s="19"/>
-      <c r="BW39" s="19"/>
-      <c r="BX39" s="19"/>
-      <c r="BY39" s="19"/>
-      <c r="BZ39" s="19"/>
-      <c r="CA39" s="19"/>
+      <c r="BJ39" s="31"/>
+      <c r="BK39" s="31"/>
+      <c r="BL39" s="31"/>
+      <c r="BM39" s="31"/>
+      <c r="BN39" s="31"/>
+      <c r="BO39" s="31"/>
+      <c r="BP39" s="14"/>
+      <c r="BQ39" s="14"/>
+      <c r="BR39" s="14"/>
+      <c r="BS39" s="14"/>
+      <c r="BT39" s="14"/>
+      <c r="BU39" s="14"/>
+      <c r="BV39" s="14"/>
+      <c r="BW39" s="14"/>
+      <c r="BX39" s="14"/>
+      <c r="BY39" s="14"/>
+      <c r="BZ39" s="14"/>
+      <c r="CA39" s="14"/>
     </row>
     <row r="40" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
@@ -2570,24 +3178,24 @@
       <c r="AE40" s="2"/>
       <c r="AF40" s="2"/>
       <c r="AG40" s="2"/>
-      <c r="BJ40" s="40"/>
-      <c r="BK40" s="40"/>
-      <c r="BL40" s="40"/>
-      <c r="BM40" s="40"/>
-      <c r="BN40" s="40"/>
-      <c r="BO40" s="40"/>
-      <c r="BP40" s="19"/>
-      <c r="BQ40" s="19"/>
-      <c r="BR40" s="19"/>
-      <c r="BS40" s="19"/>
-      <c r="BT40" s="19"/>
-      <c r="BU40" s="19"/>
-      <c r="BV40" s="19"/>
-      <c r="BW40" s="19"/>
-      <c r="BX40" s="19"/>
-      <c r="BY40" s="19"/>
-      <c r="BZ40" s="19"/>
-      <c r="CA40" s="19"/>
+      <c r="BJ40" s="31"/>
+      <c r="BK40" s="31"/>
+      <c r="BL40" s="31"/>
+      <c r="BM40" s="31"/>
+      <c r="BN40" s="31"/>
+      <c r="BO40" s="31"/>
+      <c r="BP40" s="14"/>
+      <c r="BQ40" s="14"/>
+      <c r="BR40" s="14"/>
+      <c r="BS40" s="14"/>
+      <c r="BT40" s="14"/>
+      <c r="BU40" s="14"/>
+      <c r="BV40" s="14"/>
+      <c r="BW40" s="14"/>
+      <c r="BX40" s="14"/>
+      <c r="BY40" s="14"/>
+      <c r="BZ40" s="14"/>
+      <c r="CA40" s="14"/>
     </row>
     <row r="41" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
@@ -2623,24 +3231,24 @@
       <c r="AE41" s="2"/>
       <c r="AF41" s="2"/>
       <c r="AG41" s="2"/>
-      <c r="BJ41" s="40"/>
-      <c r="BK41" s="40"/>
-      <c r="BL41" s="40"/>
-      <c r="BM41" s="40"/>
-      <c r="BN41" s="40"/>
-      <c r="BO41" s="40"/>
-      <c r="BP41" s="19"/>
-      <c r="BQ41" s="19"/>
-      <c r="BR41" s="19"/>
-      <c r="BS41" s="19"/>
-      <c r="BT41" s="19"/>
-      <c r="BU41" s="19"/>
-      <c r="BV41" s="19"/>
-      <c r="BW41" s="19"/>
-      <c r="BX41" s="19"/>
-      <c r="BY41" s="19"/>
-      <c r="BZ41" s="19"/>
-      <c r="CA41" s="19"/>
+      <c r="BJ41" s="31"/>
+      <c r="BK41" s="31"/>
+      <c r="BL41" s="31"/>
+      <c r="BM41" s="31"/>
+      <c r="BN41" s="31"/>
+      <c r="BO41" s="31"/>
+      <c r="BP41" s="14"/>
+      <c r="BQ41" s="14"/>
+      <c r="BR41" s="14"/>
+      <c r="BS41" s="14"/>
+      <c r="BT41" s="14"/>
+      <c r="BU41" s="14"/>
+      <c r="BV41" s="14"/>
+      <c r="BW41" s="14"/>
+      <c r="BX41" s="14"/>
+      <c r="BY41" s="14"/>
+      <c r="BZ41" s="14"/>
+      <c r="CA41" s="14"/>
     </row>
     <row r="42" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
@@ -2676,24 +3284,24 @@
       <c r="AE42" s="2"/>
       <c r="AF42" s="2"/>
       <c r="AG42" s="2"/>
-      <c r="BJ42" s="40"/>
-      <c r="BK42" s="40"/>
-      <c r="BL42" s="40"/>
-      <c r="BM42" s="40"/>
-      <c r="BN42" s="40"/>
-      <c r="BO42" s="40"/>
-      <c r="BP42" s="19"/>
-      <c r="BQ42" s="19"/>
-      <c r="BR42" s="19"/>
-      <c r="BS42" s="19"/>
-      <c r="BT42" s="19"/>
-      <c r="BU42" s="19"/>
-      <c r="BV42" s="19"/>
-      <c r="BW42" s="19"/>
-      <c r="BX42" s="19"/>
-      <c r="BY42" s="19"/>
-      <c r="BZ42" s="19"/>
-      <c r="CA42" s="19"/>
+      <c r="BJ42" s="31"/>
+      <c r="BK42" s="31"/>
+      <c r="BL42" s="31"/>
+      <c r="BM42" s="31"/>
+      <c r="BN42" s="31"/>
+      <c r="BO42" s="31"/>
+      <c r="BP42" s="14"/>
+      <c r="BQ42" s="14"/>
+      <c r="BR42" s="14"/>
+      <c r="BS42" s="14"/>
+      <c r="BT42" s="14"/>
+      <c r="BU42" s="14"/>
+      <c r="BV42" s="14"/>
+      <c r="BW42" s="14"/>
+      <c r="BX42" s="14"/>
+      <c r="BY42" s="14"/>
+      <c r="BZ42" s="14"/>
+      <c r="CA42" s="14"/>
     </row>
     <row r="43" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
@@ -2729,24 +3337,24 @@
       <c r="AE43" s="2"/>
       <c r="AF43" s="2"/>
       <c r="AG43" s="2"/>
-      <c r="BJ43" s="40"/>
-      <c r="BK43" s="40"/>
-      <c r="BL43" s="40"/>
-      <c r="BM43" s="40"/>
-      <c r="BN43" s="40"/>
-      <c r="BO43" s="40"/>
-      <c r="BP43" s="19"/>
-      <c r="BQ43" s="19"/>
-      <c r="BR43" s="19"/>
-      <c r="BS43" s="19"/>
-      <c r="BT43" s="19"/>
-      <c r="BU43" s="19"/>
-      <c r="BV43" s="19"/>
-      <c r="BW43" s="19"/>
-      <c r="BX43" s="19"/>
-      <c r="BY43" s="19"/>
-      <c r="BZ43" s="19"/>
-      <c r="CA43" s="19"/>
+      <c r="BJ43" s="31"/>
+      <c r="BK43" s="31"/>
+      <c r="BL43" s="31"/>
+      <c r="BM43" s="31"/>
+      <c r="BN43" s="31"/>
+      <c r="BO43" s="31"/>
+      <c r="BP43" s="14"/>
+      <c r="BQ43" s="14"/>
+      <c r="BR43" s="14"/>
+      <c r="BS43" s="14"/>
+      <c r="BT43" s="14"/>
+      <c r="BU43" s="14"/>
+      <c r="BV43" s="14"/>
+      <c r="BW43" s="14"/>
+      <c r="BX43" s="14"/>
+      <c r="BY43" s="14"/>
+      <c r="BZ43" s="14"/>
+      <c r="CA43" s="14"/>
     </row>
     <row r="44" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
@@ -2782,24 +3390,24 @@
       <c r="AE44" s="2"/>
       <c r="AF44" s="2"/>
       <c r="AG44" s="2"/>
-      <c r="BJ44" s="40"/>
-      <c r="BK44" s="40"/>
-      <c r="BL44" s="40"/>
-      <c r="BM44" s="40"/>
-      <c r="BN44" s="40"/>
-      <c r="BO44" s="40"/>
-      <c r="BP44" s="19"/>
-      <c r="BQ44" s="19"/>
-      <c r="BR44" s="19"/>
-      <c r="BS44" s="19"/>
-      <c r="BT44" s="19"/>
-      <c r="BU44" s="19"/>
-      <c r="BV44" s="19"/>
-      <c r="BW44" s="19"/>
-      <c r="BX44" s="19"/>
-      <c r="BY44" s="19"/>
-      <c r="BZ44" s="19"/>
-      <c r="CA44" s="19"/>
+      <c r="BJ44" s="31"/>
+      <c r="BK44" s="31"/>
+      <c r="BL44" s="31"/>
+      <c r="BM44" s="31"/>
+      <c r="BN44" s="31"/>
+      <c r="BO44" s="31"/>
+      <c r="BP44" s="14"/>
+      <c r="BQ44" s="14"/>
+      <c r="BR44" s="14"/>
+      <c r="BS44" s="14"/>
+      <c r="BT44" s="14"/>
+      <c r="BU44" s="14"/>
+      <c r="BV44" s="14"/>
+      <c r="BW44" s="14"/>
+      <c r="BX44" s="14"/>
+      <c r="BY44" s="14"/>
+      <c r="BZ44" s="14"/>
+      <c r="CA44" s="14"/>
     </row>
     <row r="45" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
@@ -2835,24 +3443,24 @@
       <c r="AE45" s="2"/>
       <c r="AF45" s="2"/>
       <c r="AG45" s="2"/>
-      <c r="BJ45" s="40"/>
-      <c r="BK45" s="40"/>
-      <c r="BL45" s="40"/>
-      <c r="BM45" s="40"/>
-      <c r="BN45" s="40"/>
-      <c r="BO45" s="40"/>
-      <c r="BP45" s="19"/>
-      <c r="BQ45" s="19"/>
-      <c r="BR45" s="19"/>
-      <c r="BS45" s="19"/>
-      <c r="BT45" s="19"/>
-      <c r="BU45" s="19"/>
-      <c r="BV45" s="19"/>
-      <c r="BW45" s="19"/>
-      <c r="BX45" s="19"/>
-      <c r="BY45" s="19"/>
-      <c r="BZ45" s="19"/>
-      <c r="CA45" s="19"/>
+      <c r="BJ45" s="31"/>
+      <c r="BK45" s="31"/>
+      <c r="BL45" s="31"/>
+      <c r="BM45" s="31"/>
+      <c r="BN45" s="31"/>
+      <c r="BO45" s="31"/>
+      <c r="BP45" s="14"/>
+      <c r="BQ45" s="14"/>
+      <c r="BR45" s="14"/>
+      <c r="BS45" s="14"/>
+      <c r="BT45" s="14"/>
+      <c r="BU45" s="14"/>
+      <c r="BV45" s="14"/>
+      <c r="BW45" s="14"/>
+      <c r="BX45" s="14"/>
+      <c r="BY45" s="14"/>
+      <c r="BZ45" s="14"/>
+      <c r="CA45" s="14"/>
     </row>
     <row r="46" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A46" s="1"/>
@@ -2888,24 +3496,24 @@
       <c r="AE46" s="2"/>
       <c r="AF46" s="2"/>
       <c r="AG46" s="2"/>
-      <c r="BJ46" s="40"/>
-      <c r="BK46" s="40"/>
-      <c r="BL46" s="40"/>
-      <c r="BM46" s="40"/>
-      <c r="BN46" s="40"/>
-      <c r="BO46" s="40"/>
-      <c r="BP46" s="19"/>
-      <c r="BQ46" s="19"/>
-      <c r="BR46" s="19"/>
-      <c r="BS46" s="19"/>
-      <c r="BT46" s="19"/>
-      <c r="BU46" s="19"/>
-      <c r="BV46" s="19"/>
-      <c r="BW46" s="19"/>
-      <c r="BX46" s="19"/>
-      <c r="BY46" s="19"/>
-      <c r="BZ46" s="19"/>
-      <c r="CA46" s="19"/>
+      <c r="BJ46" s="31"/>
+      <c r="BK46" s="31"/>
+      <c r="BL46" s="31"/>
+      <c r="BM46" s="31"/>
+      <c r="BN46" s="31"/>
+      <c r="BO46" s="31"/>
+      <c r="BP46" s="14"/>
+      <c r="BQ46" s="14"/>
+      <c r="BR46" s="14"/>
+      <c r="BS46" s="14"/>
+      <c r="BT46" s="14"/>
+      <c r="BU46" s="14"/>
+      <c r="BV46" s="14"/>
+      <c r="BW46" s="14"/>
+      <c r="BX46" s="14"/>
+      <c r="BY46" s="14"/>
+      <c r="BZ46" s="14"/>
+      <c r="CA46" s="14"/>
     </row>
     <row r="47" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A47" s="1"/>
@@ -2941,24 +3549,24 @@
       <c r="AE47" s="2"/>
       <c r="AF47" s="2"/>
       <c r="AG47" s="2"/>
-      <c r="BJ47" s="40"/>
-      <c r="BK47" s="40"/>
-      <c r="BL47" s="40"/>
-      <c r="BM47" s="40"/>
-      <c r="BN47" s="40"/>
-      <c r="BO47" s="40"/>
-      <c r="BP47" s="19"/>
-      <c r="BQ47" s="19"/>
-      <c r="BR47" s="19"/>
-      <c r="BS47" s="19"/>
-      <c r="BT47" s="19"/>
-      <c r="BU47" s="19"/>
-      <c r="BV47" s="19"/>
-      <c r="BW47" s="19"/>
-      <c r="BX47" s="19"/>
-      <c r="BY47" s="19"/>
-      <c r="BZ47" s="19"/>
-      <c r="CA47" s="19"/>
+      <c r="BJ47" s="31"/>
+      <c r="BK47" s="31"/>
+      <c r="BL47" s="31"/>
+      <c r="BM47" s="31"/>
+      <c r="BN47" s="31"/>
+      <c r="BO47" s="31"/>
+      <c r="BP47" s="14"/>
+      <c r="BQ47" s="14"/>
+      <c r="BR47" s="14"/>
+      <c r="BS47" s="14"/>
+      <c r="BT47" s="14"/>
+      <c r="BU47" s="14"/>
+      <c r="BV47" s="14"/>
+      <c r="BW47" s="14"/>
+      <c r="BX47" s="14"/>
+      <c r="BY47" s="14"/>
+      <c r="BZ47" s="14"/>
+      <c r="CA47" s="14"/>
     </row>
     <row r="48" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A48" s="1"/>
@@ -2967,10 +3575,10 @@
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
-      <c r="G48" s="12"/>
-      <c r="H48" s="12"/>
-      <c r="I48" s="12"/>
-      <c r="J48" s="12"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
       <c r="K48" s="7"/>
       <c r="L48" s="7"/>
       <c r="M48" s="8"/>
@@ -2994,24 +3602,24 @@
       <c r="AE48" s="2"/>
       <c r="AF48" s="2"/>
       <c r="AG48" s="2"/>
-      <c r="BJ48" s="40"/>
-      <c r="BK48" s="40"/>
-      <c r="BL48" s="40"/>
-      <c r="BM48" s="40"/>
-      <c r="BN48" s="40"/>
-      <c r="BO48" s="40"/>
-      <c r="BP48" s="19"/>
-      <c r="BQ48" s="19"/>
-      <c r="BR48" s="19"/>
-      <c r="BS48" s="19"/>
-      <c r="BT48" s="19"/>
-      <c r="BU48" s="19"/>
-      <c r="BV48" s="19"/>
-      <c r="BW48" s="19"/>
-      <c r="BX48" s="19"/>
-      <c r="BY48" s="19"/>
-      <c r="BZ48" s="19"/>
-      <c r="CA48" s="19"/>
+      <c r="BJ48" s="31"/>
+      <c r="BK48" s="31"/>
+      <c r="BL48" s="31"/>
+      <c r="BM48" s="31"/>
+      <c r="BN48" s="31"/>
+      <c r="BO48" s="31"/>
+      <c r="BP48" s="14"/>
+      <c r="BQ48" s="14"/>
+      <c r="BR48" s="14"/>
+      <c r="BS48" s="14"/>
+      <c r="BT48" s="14"/>
+      <c r="BU48" s="14"/>
+      <c r="BV48" s="14"/>
+      <c r="BW48" s="14"/>
+      <c r="BX48" s="14"/>
+      <c r="BY48" s="14"/>
+      <c r="BZ48" s="14"/>
+      <c r="CA48" s="14"/>
     </row>
     <row r="49" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A49" s="1"/>
@@ -3020,10 +3628,10 @@
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
-      <c r="G49" s="12"/>
-      <c r="H49" s="12"/>
-      <c r="I49" s="12"/>
-      <c r="J49" s="12"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="11"/>
       <c r="K49" s="8"/>
       <c r="L49" s="8"/>
       <c r="M49" s="8"/>
@@ -3047,24 +3655,24 @@
       <c r="AE49" s="2"/>
       <c r="AF49" s="2"/>
       <c r="AG49" s="2"/>
-      <c r="BJ49" s="40"/>
-      <c r="BK49" s="40"/>
-      <c r="BL49" s="40"/>
-      <c r="BM49" s="40"/>
-      <c r="BN49" s="40"/>
-      <c r="BO49" s="40"/>
-      <c r="BP49" s="19"/>
-      <c r="BQ49" s="19"/>
-      <c r="BR49" s="19"/>
-      <c r="BS49" s="19"/>
-      <c r="BT49" s="19"/>
-      <c r="BU49" s="19"/>
-      <c r="BV49" s="19"/>
-      <c r="BW49" s="19"/>
-      <c r="BX49" s="19"/>
-      <c r="BY49" s="19"/>
-      <c r="BZ49" s="19"/>
-      <c r="CA49" s="19"/>
+      <c r="BJ49" s="31"/>
+      <c r="BK49" s="31"/>
+      <c r="BL49" s="31"/>
+      <c r="BM49" s="31"/>
+      <c r="BN49" s="31"/>
+      <c r="BO49" s="31"/>
+      <c r="BP49" s="14"/>
+      <c r="BQ49" s="14"/>
+      <c r="BR49" s="14"/>
+      <c r="BS49" s="14"/>
+      <c r="BT49" s="14"/>
+      <c r="BU49" s="14"/>
+      <c r="BV49" s="14"/>
+      <c r="BW49" s="14"/>
+      <c r="BX49" s="14"/>
+      <c r="BY49" s="14"/>
+      <c r="BZ49" s="14"/>
+      <c r="CA49" s="14"/>
     </row>
     <row r="50" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A50" s="1"/>
@@ -3073,16 +3681,16 @@
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="12"/>
-      <c r="I50" s="12"/>
-      <c r="J50" s="12"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
       <c r="K50" s="7"/>
       <c r="L50" s="7"/>
       <c r="M50" s="8"/>
       <c r="N50" s="8"/>
       <c r="O50" s="8"/>
-      <c r="P50" s="14"/>
+      <c r="P50" s="12"/>
       <c r="Q50" s="8"/>
       <c r="R50" s="8"/>
       <c r="S50" s="8"/>
@@ -3100,24 +3708,24 @@
       <c r="AE50" s="2"/>
       <c r="AF50" s="2"/>
       <c r="AG50" s="2"/>
-      <c r="BJ50" s="40"/>
-      <c r="BK50" s="40"/>
-      <c r="BL50" s="40"/>
-      <c r="BM50" s="40"/>
-      <c r="BN50" s="40"/>
-      <c r="BO50" s="40"/>
-      <c r="BP50" s="19"/>
-      <c r="BQ50" s="19"/>
-      <c r="BR50" s="19"/>
-      <c r="BS50" s="19"/>
-      <c r="BT50" s="19"/>
-      <c r="BU50" s="19"/>
-      <c r="BV50" s="19"/>
-      <c r="BW50" s="19"/>
-      <c r="BX50" s="19"/>
-      <c r="BY50" s="19"/>
-      <c r="BZ50" s="19"/>
-      <c r="CA50" s="19"/>
+      <c r="BJ50" s="31"/>
+      <c r="BK50" s="31"/>
+      <c r="BL50" s="31"/>
+      <c r="BM50" s="31"/>
+      <c r="BN50" s="31"/>
+      <c r="BO50" s="31"/>
+      <c r="BP50" s="14"/>
+      <c r="BQ50" s="14"/>
+      <c r="BR50" s="14"/>
+      <c r="BS50" s="14"/>
+      <c r="BT50" s="14"/>
+      <c r="BU50" s="14"/>
+      <c r="BV50" s="14"/>
+      <c r="BW50" s="14"/>
+      <c r="BX50" s="14"/>
+      <c r="BY50" s="14"/>
+      <c r="BZ50" s="14"/>
+      <c r="CA50" s="14"/>
     </row>
     <row r="51" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A51" s="1"/>
@@ -3126,10 +3734,10 @@
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
-      <c r="G51" s="12"/>
-      <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
-      <c r="J51" s="12"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
       <c r="K51" s="8"/>
       <c r="L51" s="8"/>
       <c r="M51" s="8"/>
@@ -3153,24 +3761,24 @@
       <c r="AE51" s="2"/>
       <c r="AF51" s="2"/>
       <c r="AG51" s="2"/>
-      <c r="BJ51" s="40"/>
-      <c r="BK51" s="40"/>
-      <c r="BL51" s="40"/>
-      <c r="BM51" s="40"/>
-      <c r="BN51" s="40"/>
-      <c r="BO51" s="40"/>
-      <c r="BP51" s="19"/>
-      <c r="BQ51" s="19"/>
-      <c r="BR51" s="19"/>
-      <c r="BS51" s="19"/>
-      <c r="BT51" s="19"/>
-      <c r="BU51" s="19"/>
-      <c r="BV51" s="19"/>
-      <c r="BW51" s="19"/>
-      <c r="BX51" s="19"/>
-      <c r="BY51" s="19"/>
-      <c r="BZ51" s="19"/>
-      <c r="CA51" s="19"/>
+      <c r="BJ51" s="31"/>
+      <c r="BK51" s="31"/>
+      <c r="BL51" s="31"/>
+      <c r="BM51" s="31"/>
+      <c r="BN51" s="31"/>
+      <c r="BO51" s="31"/>
+      <c r="BP51" s="14"/>
+      <c r="BQ51" s="14"/>
+      <c r="BR51" s="14"/>
+      <c r="BS51" s="14"/>
+      <c r="BT51" s="14"/>
+      <c r="BU51" s="14"/>
+      <c r="BV51" s="14"/>
+      <c r="BW51" s="14"/>
+      <c r="BX51" s="14"/>
+      <c r="BY51" s="14"/>
+      <c r="BZ51" s="14"/>
+      <c r="CA51" s="14"/>
     </row>
     <row r="52" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A52" s="1"/>
@@ -3179,10 +3787,10 @@
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
-      <c r="G52" s="12"/>
-      <c r="H52" s="12"/>
-      <c r="I52" s="12"/>
-      <c r="J52" s="12"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="11"/>
       <c r="K52" s="7"/>
       <c r="L52" s="7"/>
       <c r="M52" s="8"/>
@@ -3206,24 +3814,24 @@
       <c r="AE52" s="2"/>
       <c r="AF52" s="2"/>
       <c r="AG52" s="2"/>
-      <c r="BJ52" s="40"/>
-      <c r="BK52" s="40"/>
-      <c r="BL52" s="40"/>
-      <c r="BM52" s="40"/>
-      <c r="BN52" s="40"/>
-      <c r="BO52" s="40"/>
-      <c r="BP52" s="19"/>
-      <c r="BQ52" s="19"/>
-      <c r="BR52" s="19"/>
-      <c r="BS52" s="19"/>
-      <c r="BT52" s="19"/>
-      <c r="BU52" s="19"/>
-      <c r="BV52" s="19"/>
-      <c r="BW52" s="19"/>
-      <c r="BX52" s="19"/>
-      <c r="BY52" s="19"/>
-      <c r="BZ52" s="19"/>
-      <c r="CA52" s="19"/>
+      <c r="BJ52" s="31"/>
+      <c r="BK52" s="31"/>
+      <c r="BL52" s="31"/>
+      <c r="BM52" s="31"/>
+      <c r="BN52" s="31"/>
+      <c r="BO52" s="31"/>
+      <c r="BP52" s="14"/>
+      <c r="BQ52" s="14"/>
+      <c r="BR52" s="14"/>
+      <c r="BS52" s="14"/>
+      <c r="BT52" s="14"/>
+      <c r="BU52" s="14"/>
+      <c r="BV52" s="14"/>
+      <c r="BW52" s="14"/>
+      <c r="BX52" s="14"/>
+      <c r="BY52" s="14"/>
+      <c r="BZ52" s="14"/>
+      <c r="CA52" s="14"/>
     </row>
     <row r="53" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A53" s="1"/>
@@ -3232,10 +3840,10 @@
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
-      <c r="G53" s="12"/>
-      <c r="H53" s="12"/>
-      <c r="I53" s="12"/>
-      <c r="J53" s="12"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="11"/>
       <c r="K53" s="8"/>
       <c r="L53" s="8"/>
       <c r="M53" s="8"/>
@@ -3259,24 +3867,24 @@
       <c r="AE53" s="2"/>
       <c r="AF53" s="2"/>
       <c r="AG53" s="2"/>
-      <c r="BJ53" s="40"/>
-      <c r="BK53" s="40"/>
-      <c r="BL53" s="40"/>
-      <c r="BM53" s="40"/>
-      <c r="BN53" s="40"/>
-      <c r="BO53" s="40"/>
-      <c r="BP53" s="19"/>
-      <c r="BQ53" s="19"/>
-      <c r="BR53" s="19"/>
-      <c r="BS53" s="19"/>
-      <c r="BT53" s="19"/>
-      <c r="BU53" s="19"/>
-      <c r="BV53" s="19"/>
-      <c r="BW53" s="19"/>
-      <c r="BX53" s="19"/>
-      <c r="BY53" s="19"/>
-      <c r="BZ53" s="19"/>
-      <c r="CA53" s="19"/>
+      <c r="BJ53" s="31"/>
+      <c r="BK53" s="31"/>
+      <c r="BL53" s="31"/>
+      <c r="BM53" s="31"/>
+      <c r="BN53" s="31"/>
+      <c r="BO53" s="31"/>
+      <c r="BP53" s="14"/>
+      <c r="BQ53" s="14"/>
+      <c r="BR53" s="14"/>
+      <c r="BS53" s="14"/>
+      <c r="BT53" s="14"/>
+      <c r="BU53" s="14"/>
+      <c r="BV53" s="14"/>
+      <c r="BW53" s="14"/>
+      <c r="BX53" s="14"/>
+      <c r="BY53" s="14"/>
+      <c r="BZ53" s="14"/>
+      <c r="CA53" s="14"/>
     </row>
     <row r="54" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A54" s="1"/>
@@ -3285,10 +3893,10 @@
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
-      <c r="G54" s="12"/>
-      <c r="H54" s="12"/>
-      <c r="I54" s="12"/>
-      <c r="J54" s="12"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="11"/>
+      <c r="J54" s="11"/>
       <c r="K54" s="7"/>
       <c r="L54" s="7"/>
       <c r="M54" s="8"/>
@@ -3312,24 +3920,24 @@
       <c r="AE54" s="2"/>
       <c r="AF54" s="2"/>
       <c r="AG54" s="2"/>
-      <c r="BJ54" s="40"/>
-      <c r="BK54" s="40"/>
-      <c r="BL54" s="40"/>
-      <c r="BM54" s="40"/>
-      <c r="BN54" s="40"/>
-      <c r="BO54" s="40"/>
-      <c r="BP54" s="19"/>
-      <c r="BQ54" s="19"/>
-      <c r="BR54" s="19"/>
-      <c r="BS54" s="19"/>
-      <c r="BT54" s="19"/>
-      <c r="BU54" s="19"/>
-      <c r="BV54" s="19"/>
-      <c r="BW54" s="19"/>
-      <c r="BX54" s="19"/>
-      <c r="BY54" s="19"/>
-      <c r="BZ54" s="19"/>
-      <c r="CA54" s="19"/>
+      <c r="BJ54" s="31"/>
+      <c r="BK54" s="31"/>
+      <c r="BL54" s="31"/>
+      <c r="BM54" s="31"/>
+      <c r="BN54" s="31"/>
+      <c r="BO54" s="31"/>
+      <c r="BP54" s="14"/>
+      <c r="BQ54" s="14"/>
+      <c r="BR54" s="14"/>
+      <c r="BS54" s="14"/>
+      <c r="BT54" s="14"/>
+      <c r="BU54" s="14"/>
+      <c r="BV54" s="14"/>
+      <c r="BW54" s="14"/>
+      <c r="BX54" s="14"/>
+      <c r="BY54" s="14"/>
+      <c r="BZ54" s="14"/>
+      <c r="CA54" s="14"/>
     </row>
     <row r="55" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A55" s="1"/>
@@ -3338,10 +3946,10 @@
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="12"/>
-      <c r="I55" s="12"/>
-      <c r="J55" s="12"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="11"/>
       <c r="K55" s="8"/>
       <c r="L55" s="8"/>
       <c r="M55" s="8"/>
@@ -3365,24 +3973,24 @@
       <c r="AE55" s="2"/>
       <c r="AF55" s="2"/>
       <c r="AG55" s="2"/>
-      <c r="BJ55" s="40"/>
-      <c r="BK55" s="40"/>
-      <c r="BL55" s="40"/>
-      <c r="BM55" s="40"/>
-      <c r="BN55" s="40"/>
-      <c r="BO55" s="40"/>
-      <c r="BP55" s="19"/>
-      <c r="BQ55" s="19"/>
-      <c r="BR55" s="19"/>
-      <c r="BS55" s="19"/>
-      <c r="BT55" s="19"/>
-      <c r="BU55" s="19"/>
-      <c r="BV55" s="19"/>
-      <c r="BW55" s="19"/>
-      <c r="BX55" s="19"/>
-      <c r="BY55" s="19"/>
-      <c r="BZ55" s="19"/>
-      <c r="CA55" s="19"/>
+      <c r="BJ55" s="31"/>
+      <c r="BK55" s="31"/>
+      <c r="BL55" s="31"/>
+      <c r="BM55" s="31"/>
+      <c r="BN55" s="31"/>
+      <c r="BO55" s="31"/>
+      <c r="BP55" s="14"/>
+      <c r="BQ55" s="14"/>
+      <c r="BR55" s="14"/>
+      <c r="BS55" s="14"/>
+      <c r="BT55" s="14"/>
+      <c r="BU55" s="14"/>
+      <c r="BV55" s="14"/>
+      <c r="BW55" s="14"/>
+      <c r="BX55" s="14"/>
+      <c r="BY55" s="14"/>
+      <c r="BZ55" s="14"/>
+      <c r="CA55" s="14"/>
     </row>
     <row r="56" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A56" s="1"/>
@@ -3391,10 +3999,10 @@
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
-      <c r="G56" s="12"/>
-      <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
-      <c r="J56" s="12"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="11"/>
       <c r="K56" s="7"/>
       <c r="L56" s="7"/>
       <c r="M56" s="8"/>
@@ -3418,24 +4026,24 @@
       <c r="AE56" s="2"/>
       <c r="AF56" s="2"/>
       <c r="AG56" s="2"/>
-      <c r="BJ56" s="40"/>
-      <c r="BK56" s="40"/>
-      <c r="BL56" s="40"/>
-      <c r="BM56" s="40"/>
-      <c r="BN56" s="40"/>
-      <c r="BO56" s="40"/>
-      <c r="BP56" s="19"/>
-      <c r="BQ56" s="19"/>
-      <c r="BR56" s="19"/>
-      <c r="BS56" s="19"/>
-      <c r="BT56" s="19"/>
-      <c r="BU56" s="19"/>
-      <c r="BV56" s="19"/>
-      <c r="BW56" s="19"/>
-      <c r="BX56" s="19"/>
-      <c r="BY56" s="19"/>
-      <c r="BZ56" s="19"/>
-      <c r="CA56" s="19"/>
+      <c r="BJ56" s="31"/>
+      <c r="BK56" s="31"/>
+      <c r="BL56" s="31"/>
+      <c r="BM56" s="31"/>
+      <c r="BN56" s="31"/>
+      <c r="BO56" s="31"/>
+      <c r="BP56" s="14"/>
+      <c r="BQ56" s="14"/>
+      <c r="BR56" s="14"/>
+      <c r="BS56" s="14"/>
+      <c r="BT56" s="14"/>
+      <c r="BU56" s="14"/>
+      <c r="BV56" s="14"/>
+      <c r="BW56" s="14"/>
+      <c r="BX56" s="14"/>
+      <c r="BY56" s="14"/>
+      <c r="BZ56" s="14"/>
+      <c r="CA56" s="14"/>
     </row>
     <row r="57" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A57" s="1"/>
@@ -3444,10 +4052,10 @@
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
       <c r="F57" s="6"/>
-      <c r="G57" s="12"/>
-      <c r="H57" s="12"/>
-      <c r="I57" s="12"/>
-      <c r="J57" s="12"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="11"/>
       <c r="K57" s="8"/>
       <c r="L57" s="8"/>
       <c r="M57" s="8"/>
@@ -3471,24 +4079,24 @@
       <c r="AE57" s="2"/>
       <c r="AF57" s="2"/>
       <c r="AG57" s="2"/>
-      <c r="BJ57" s="19"/>
-      <c r="BK57" s="19"/>
-      <c r="BL57" s="19"/>
-      <c r="BM57" s="19"/>
-      <c r="BN57" s="19"/>
-      <c r="BO57" s="19"/>
-      <c r="BP57" s="19"/>
-      <c r="BQ57" s="19"/>
-      <c r="BR57" s="19"/>
-      <c r="BS57" s="19"/>
-      <c r="BT57" s="19"/>
-      <c r="BU57" s="19"/>
-      <c r="BV57" s="19"/>
-      <c r="BW57" s="19"/>
-      <c r="BX57" s="19"/>
-      <c r="BY57" s="19"/>
-      <c r="BZ57" s="19"/>
-      <c r="CA57" s="19"/>
+      <c r="BJ57" s="14"/>
+      <c r="BK57" s="14"/>
+      <c r="BL57" s="14"/>
+      <c r="BM57" s="14"/>
+      <c r="BN57" s="14"/>
+      <c r="BO57" s="14"/>
+      <c r="BP57" s="14"/>
+      <c r="BQ57" s="14"/>
+      <c r="BR57" s="14"/>
+      <c r="BS57" s="14"/>
+      <c r="BT57" s="14"/>
+      <c r="BU57" s="14"/>
+      <c r="BV57" s="14"/>
+      <c r="BW57" s="14"/>
+      <c r="BX57" s="14"/>
+      <c r="BY57" s="14"/>
+      <c r="BZ57" s="14"/>
+      <c r="CA57" s="14"/>
     </row>
     <row r="58" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A58" s="1"/>
@@ -3497,10 +4105,10 @@
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
       <c r="F58" s="6"/>
-      <c r="G58" s="12"/>
-      <c r="H58" s="12"/>
-      <c r="I58" s="12"/>
-      <c r="J58" s="12"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="11"/>
+      <c r="J58" s="11"/>
       <c r="K58" s="7"/>
       <c r="L58" s="7"/>
       <c r="M58" s="8"/>
@@ -3508,7 +4116,7 @@
       <c r="O58" s="8"/>
       <c r="P58" s="8"/>
       <c r="Q58" s="8"/>
-      <c r="R58" s="14"/>
+      <c r="R58" s="12"/>
       <c r="S58" s="8"/>
       <c r="T58" s="8"/>
       <c r="U58" s="2"/>
@@ -3532,10 +4140,10 @@
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
-      <c r="G59" s="12"/>
-      <c r="H59" s="12"/>
-      <c r="I59" s="12"/>
-      <c r="J59" s="12"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="11"/>
+      <c r="J59" s="11"/>
       <c r="K59" s="8"/>
       <c r="L59" s="8"/>
       <c r="M59" s="8"/>
@@ -3567,10 +4175,10 @@
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
       <c r="F60" s="6"/>
-      <c r="G60" s="12"/>
-      <c r="H60" s="12"/>
-      <c r="I60" s="12"/>
-      <c r="J60" s="12"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="11"/>
       <c r="K60" s="7"/>
       <c r="L60" s="7"/>
       <c r="M60" s="8"/>
@@ -3602,10 +4210,10 @@
       <c r="D61" s="6"/>
       <c r="E61" s="6"/>
       <c r="F61" s="6"/>
-      <c r="G61" s="12"/>
-      <c r="H61" s="12"/>
-      <c r="I61" s="12"/>
-      <c r="J61" s="12"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="11"/>
+      <c r="I61" s="11"/>
+      <c r="J61" s="11"/>
       <c r="K61" s="8"/>
       <c r="L61" s="8"/>
       <c r="M61" s="8"/>
@@ -3637,10 +4245,10 @@
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
-      <c r="G62" s="12"/>
-      <c r="H62" s="12"/>
-      <c r="I62" s="12"/>
-      <c r="J62" s="12"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
+      <c r="I62" s="11"/>
+      <c r="J62" s="11"/>
       <c r="K62" s="7"/>
       <c r="L62" s="7"/>
       <c r="M62" s="8"/>
@@ -3672,10 +4280,10 @@
       <c r="D63" s="6"/>
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
-      <c r="G63" s="12"/>
-      <c r="H63" s="12"/>
-      <c r="I63" s="12"/>
-      <c r="J63" s="12"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
+      <c r="I63" s="11"/>
+      <c r="J63" s="11"/>
       <c r="K63" s="8"/>
       <c r="L63" s="8"/>
       <c r="M63" s="8"/>
@@ -3707,10 +4315,10 @@
       <c r="D64" s="6"/>
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
-      <c r="G64" s="12"/>
-      <c r="H64" s="12"/>
-      <c r="I64" s="12"/>
-      <c r="J64" s="12"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="11"/>
       <c r="K64" s="7"/>
       <c r="L64" s="7"/>
       <c r="M64" s="8"/>
@@ -3742,10 +4350,10 @@
       <c r="D65" s="6"/>
       <c r="E65" s="6"/>
       <c r="F65" s="6"/>
-      <c r="G65" s="12"/>
-      <c r="H65" s="12"/>
-      <c r="I65" s="12"/>
-      <c r="J65" s="12"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11"/>
+      <c r="I65" s="11"/>
+      <c r="J65" s="11"/>
       <c r="K65" s="8"/>
       <c r="L65" s="8"/>
       <c r="M65" s="8"/>
@@ -3987,10 +4595,10 @@
       <c r="D72" s="6"/>
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
-      <c r="G72" s="12"/>
-      <c r="H72" s="12"/>
-      <c r="I72" s="12"/>
-      <c r="J72" s="12"/>
+      <c r="G72" s="11"/>
+      <c r="H72" s="11"/>
+      <c r="I72" s="11"/>
+      <c r="J72" s="11"/>
       <c r="K72" s="7"/>
       <c r="L72" s="7"/>
       <c r="M72" s="8"/>
@@ -4022,10 +4630,10 @@
       <c r="D73" s="6"/>
       <c r="E73" s="6"/>
       <c r="F73" s="6"/>
-      <c r="G73" s="12"/>
-      <c r="H73" s="12"/>
-      <c r="I73" s="12"/>
-      <c r="J73" s="12"/>
+      <c r="G73" s="11"/>
+      <c r="H73" s="11"/>
+      <c r="I73" s="11"/>
+      <c r="J73" s="11"/>
       <c r="K73" s="7"/>
       <c r="L73" s="7"/>
       <c r="M73" s="8"/>
@@ -4057,16 +4665,16 @@
       <c r="D74" s="6"/>
       <c r="E74" s="6"/>
       <c r="F74" s="6"/>
-      <c r="G74" s="12"/>
-      <c r="H74" s="12"/>
-      <c r="I74" s="12"/>
-      <c r="J74" s="12"/>
+      <c r="G74" s="11"/>
+      <c r="H74" s="11"/>
+      <c r="I74" s="11"/>
+      <c r="J74" s="11"/>
       <c r="K74" s="7"/>
       <c r="L74" s="7"/>
       <c r="M74" s="8"/>
       <c r="N74" s="8"/>
       <c r="O74" s="8"/>
-      <c r="P74" s="14"/>
+      <c r="P74" s="12"/>
       <c r="Q74" s="8"/>
       <c r="R74" s="8"/>
       <c r="S74" s="8"/>
@@ -4092,10 +4700,10 @@
       <c r="D75" s="6"/>
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
-      <c r="G75" s="12"/>
-      <c r="H75" s="12"/>
-      <c r="I75" s="12"/>
-      <c r="J75" s="12"/>
+      <c r="G75" s="11"/>
+      <c r="H75" s="11"/>
+      <c r="I75" s="11"/>
+      <c r="J75" s="11"/>
       <c r="K75" s="7"/>
       <c r="L75" s="7"/>
       <c r="M75" s="8"/>
@@ -4127,10 +4735,10 @@
       <c r="D76" s="6"/>
       <c r="E76" s="6"/>
       <c r="F76" s="6"/>
-      <c r="G76" s="12"/>
-      <c r="H76" s="12"/>
-      <c r="I76" s="12"/>
-      <c r="J76" s="12"/>
+      <c r="G76" s="11"/>
+      <c r="H76" s="11"/>
+      <c r="I76" s="11"/>
+      <c r="J76" s="11"/>
       <c r="K76" s="7"/>
       <c r="L76" s="7"/>
       <c r="M76" s="8"/>
@@ -4162,10 +4770,10 @@
       <c r="D77" s="6"/>
       <c r="E77" s="6"/>
       <c r="F77" s="6"/>
-      <c r="G77" s="12"/>
-      <c r="H77" s="12"/>
-      <c r="I77" s="12"/>
-      <c r="J77" s="12"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="11"/>
+      <c r="I77" s="11"/>
+      <c r="J77" s="11"/>
       <c r="K77" s="7"/>
       <c r="L77" s="7"/>
       <c r="M77" s="8"/>
@@ -4197,10 +4805,10 @@
       <c r="D78" s="6"/>
       <c r="E78" s="6"/>
       <c r="F78" s="6"/>
-      <c r="G78" s="12"/>
-      <c r="H78" s="12"/>
-      <c r="I78" s="12"/>
-      <c r="J78" s="12"/>
+      <c r="G78" s="11"/>
+      <c r="H78" s="11"/>
+      <c r="I78" s="11"/>
+      <c r="J78" s="11"/>
       <c r="K78" s="7"/>
       <c r="L78" s="7"/>
       <c r="M78" s="8"/>
@@ -4232,10 +4840,10 @@
       <c r="D79" s="6"/>
       <c r="E79" s="6"/>
       <c r="F79" s="6"/>
-      <c r="G79" s="12"/>
-      <c r="H79" s="12"/>
-      <c r="I79" s="12"/>
-      <c r="J79" s="12"/>
+      <c r="G79" s="11"/>
+      <c r="H79" s="11"/>
+      <c r="I79" s="11"/>
+      <c r="J79" s="11"/>
       <c r="K79" s="7"/>
       <c r="L79" s="7"/>
       <c r="M79" s="8"/>
@@ -4267,10 +4875,10 @@
       <c r="D80" s="6"/>
       <c r="E80" s="6"/>
       <c r="F80" s="6"/>
-      <c r="G80" s="12"/>
-      <c r="H80" s="12"/>
-      <c r="I80" s="12"/>
-      <c r="J80" s="12"/>
+      <c r="G80" s="11"/>
+      <c r="H80" s="11"/>
+      <c r="I80" s="11"/>
+      <c r="J80" s="11"/>
       <c r="K80" s="7"/>
       <c r="L80" s="7"/>
       <c r="M80" s="8"/>
@@ -4302,10 +4910,10 @@
       <c r="D81" s="6"/>
       <c r="E81" s="6"/>
       <c r="F81" s="6"/>
-      <c r="G81" s="12"/>
-      <c r="H81" s="12"/>
-      <c r="I81" s="12"/>
-      <c r="J81" s="12"/>
+      <c r="G81" s="11"/>
+      <c r="H81" s="11"/>
+      <c r="I81" s="11"/>
+      <c r="J81" s="11"/>
       <c r="K81" s="7"/>
       <c r="L81" s="7"/>
       <c r="M81" s="8"/>
@@ -4337,10 +4945,10 @@
       <c r="D82" s="6"/>
       <c r="E82" s="6"/>
       <c r="F82" s="6"/>
-      <c r="G82" s="12"/>
-      <c r="H82" s="12"/>
-      <c r="I82" s="12"/>
-      <c r="J82" s="12"/>
+      <c r="G82" s="11"/>
+      <c r="H82" s="11"/>
+      <c r="I82" s="11"/>
+      <c r="J82" s="11"/>
       <c r="K82" s="7"/>
       <c r="L82" s="7"/>
       <c r="M82" s="8"/>
@@ -4348,7 +4956,7 @@
       <c r="O82" s="8"/>
       <c r="P82" s="8"/>
       <c r="Q82" s="8"/>
-      <c r="R82" s="14"/>
+      <c r="R82" s="12"/>
       <c r="S82" s="8"/>
       <c r="T82" s="8"/>
       <c r="U82" s="2"/>
@@ -4372,10 +4980,10 @@
       <c r="D83" s="6"/>
       <c r="E83" s="6"/>
       <c r="F83" s="6"/>
-      <c r="G83" s="12"/>
-      <c r="H83" s="12"/>
-      <c r="I83" s="12"/>
-      <c r="J83" s="12"/>
+      <c r="G83" s="11"/>
+      <c r="H83" s="11"/>
+      <c r="I83" s="11"/>
+      <c r="J83" s="11"/>
       <c r="K83" s="7"/>
       <c r="L83" s="7"/>
       <c r="M83" s="8"/>
@@ -4407,10 +5015,10 @@
       <c r="D84" s="6"/>
       <c r="E84" s="6"/>
       <c r="F84" s="6"/>
-      <c r="G84" s="12"/>
-      <c r="H84" s="12"/>
-      <c r="I84" s="12"/>
-      <c r="J84" s="12"/>
+      <c r="G84" s="11"/>
+      <c r="H84" s="11"/>
+      <c r="I84" s="11"/>
+      <c r="J84" s="11"/>
       <c r="K84" s="7"/>
       <c r="L84" s="7"/>
       <c r="M84" s="8"/>
@@ -4442,10 +5050,10 @@
       <c r="D85" s="6"/>
       <c r="E85" s="6"/>
       <c r="F85" s="6"/>
-      <c r="G85" s="12"/>
-      <c r="H85" s="12"/>
-      <c r="I85" s="12"/>
-      <c r="J85" s="12"/>
+      <c r="G85" s="11"/>
+      <c r="H85" s="11"/>
+      <c r="I85" s="11"/>
+      <c r="J85" s="11"/>
       <c r="K85" s="7"/>
       <c r="L85" s="7"/>
       <c r="M85" s="8"/>
@@ -4477,10 +5085,10 @@
       <c r="D86" s="6"/>
       <c r="E86" s="6"/>
       <c r="F86" s="6"/>
-      <c r="G86" s="12"/>
-      <c r="H86" s="12"/>
-      <c r="I86" s="12"/>
-      <c r="J86" s="12"/>
+      <c r="G86" s="11"/>
+      <c r="H86" s="11"/>
+      <c r="I86" s="11"/>
+      <c r="J86" s="11"/>
       <c r="K86" s="7"/>
       <c r="L86" s="7"/>
       <c r="M86" s="8"/>
@@ -4510,10 +5118,10 @@
       <c r="D87" s="6"/>
       <c r="E87" s="6"/>
       <c r="F87" s="6"/>
-      <c r="G87" s="12"/>
-      <c r="H87" s="12"/>
-      <c r="I87" s="12"/>
-      <c r="J87" s="12"/>
+      <c r="G87" s="11"/>
+      <c r="H87" s="11"/>
+      <c r="I87" s="11"/>
+      <c r="J87" s="11"/>
       <c r="K87" s="7"/>
       <c r="L87" s="7"/>
       <c r="M87" s="8"/>
@@ -4543,10 +5151,10 @@
       <c r="D88" s="6"/>
       <c r="E88" s="6"/>
       <c r="F88" s="6"/>
-      <c r="G88" s="12"/>
-      <c r="H88" s="12"/>
-      <c r="I88" s="12"/>
-      <c r="J88" s="12"/>
+      <c r="G88" s="11"/>
+      <c r="H88" s="11"/>
+      <c r="I88" s="11"/>
+      <c r="J88" s="11"/>
       <c r="K88" s="7"/>
       <c r="L88" s="7"/>
       <c r="M88" s="8"/>
@@ -4576,10 +5184,10 @@
       <c r="D89" s="6"/>
       <c r="E89" s="6"/>
       <c r="F89" s="6"/>
-      <c r="G89" s="12"/>
-      <c r="H89" s="12"/>
-      <c r="I89" s="12"/>
-      <c r="J89" s="12"/>
+      <c r="G89" s="11"/>
+      <c r="H89" s="11"/>
+      <c r="I89" s="11"/>
+      <c r="J89" s="11"/>
       <c r="K89" s="7"/>
       <c r="L89" s="7"/>
       <c r="M89" s="8"/>
@@ -5647,18 +6255,17 @@
       <c r="AC128" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="8">
+    <mergeCell ref="D3:T4"/>
+    <mergeCell ref="D2:T2"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="BJ34:BO56"/>
-    <mergeCell ref="E24:F24"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="E29:F29"/>
-    <mergeCell ref="D2:Z2"/>
-    <mergeCell ref="D3:Z4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="14" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>